<commit_message>
update clean+merge for seagrass+epiphytes
- added corrected data from 2017 and 2018
- changed calculation of shoot and epiphyte biomass based on knowledge of column names
</commit_message>
<xml_diff>
--- a/metadata/O'Connor_Parfrey_data_coverage.xlsx
+++ b/metadata/O'Connor_Parfrey_data_coverage.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\O'Connor Data\Calvert_O'Connor_eelgrass\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\O'Connor Data\Calvert_O'Connor_eelgrass\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D32D2-9E48-46CA-83FC-771F4E4E3723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F575FD43-E187-472C-9A61-46B6666BD3ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{5ABB7252-36D3-4718-9F6B-605ABC616F06}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15300" windowHeight="7875" xr2:uid="{5ABB7252-36D3-4718-9F6B-605ABC616F06}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="measurement_year" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>year</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>microbes</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABFEBD-98B2-437C-A76A-3BE2B8961C31}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +417,7 @@
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +433,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2014</v>
       </c>
@@ -448,7 +454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -464,8 +470,11 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -481,8 +490,11 @@
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -498,8 +510,11 @@
       <c r="E5">
         <v>5</v>
       </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -514,6 +529,9 @@
       </c>
       <c r="E6">
         <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>